<commit_message>
Presentation and updated budget
</commit_message>
<xml_diff>
--- a/documentation/Budget.xlsx
+++ b/documentation/Budget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\humber.org\home\03\0118\n01183879\Semester 5\CENG 317 - Hardware Production Tech\Digole-LCD-Display\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Semester 5\CENG 317 - Hardware Production Tech\Digole-LCD-Display\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -186,9 +186,6 @@
   </si>
   <si>
     <t>√</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>Total Owned</t>
@@ -218,7 +215,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -428,20 +425,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -456,23 +453,23 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -486,13 +483,13 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -516,19 +513,19 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="10" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="11" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="8" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -824,8 +821,8 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -845,7 +842,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="18">
       <c r="A1" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="42"/>
     </row>
@@ -988,7 +985,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="20">
-        <f>E5*0.13</f>
+        <f t="shared" ref="H5:H14" si="0">E5*0.13</f>
         <v>0.64870000000000005</v>
       </c>
       <c r="I5" s="20">
@@ -998,7 +995,7 @@
         <v>8.99</v>
       </c>
       <c r="K5" s="20">
-        <f>E5+H5+J5</f>
+        <f t="shared" ref="K5:K12" si="1">E5+H5+J5</f>
         <v>14.6287</v>
       </c>
       <c r="L5" s="34" t="s">
@@ -1028,7 +1025,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="17">
-        <f>E6*0.13</f>
+        <f t="shared" si="0"/>
         <v>0.32500000000000001</v>
       </c>
       <c r="I6" s="17">
@@ -1038,7 +1035,7 @@
         <v>4.74</v>
       </c>
       <c r="K6" s="17">
-        <f>E6+H6+J6</f>
+        <f t="shared" si="1"/>
         <v>7.5650000000000004</v>
       </c>
       <c r="L6" s="35" t="s">
@@ -1068,7 +1065,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="20">
-        <f>E7*0.13</f>
+        <f t="shared" si="0"/>
         <v>0.32500000000000001</v>
       </c>
       <c r="I7" s="20">
@@ -1078,7 +1075,7 @@
         <v>4.74</v>
       </c>
       <c r="K7" s="20">
-        <f>E7+H7+J7</f>
+        <f t="shared" si="1"/>
         <v>7.5650000000000004</v>
       </c>
       <c r="L7" s="34" t="s">
@@ -1108,7 +1105,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="17">
-        <f>E8*0.13</f>
+        <f t="shared" si="0"/>
         <v>0.77350000000000008</v>
       </c>
       <c r="I8" s="17">
@@ -1118,7 +1115,7 @@
         <v>4.74</v>
       </c>
       <c r="K8" s="17">
-        <f>E8+H8+J8</f>
+        <f t="shared" si="1"/>
         <v>11.4635</v>
       </c>
       <c r="L8" s="35" t="s">
@@ -1148,7 +1145,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="20">
-        <f>E9*0.13</f>
+        <f t="shared" si="0"/>
         <v>3.6387</v>
       </c>
       <c r="I9" s="20">
@@ -1158,7 +1155,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="20">
-        <f>E9+H9+J9</f>
+        <f t="shared" si="1"/>
         <v>31.628699999999998</v>
       </c>
       <c r="L9" s="34" t="s">
@@ -1188,7 +1185,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="17">
-        <f>E10*0.13</f>
+        <f t="shared" si="0"/>
         <v>15.600000000000001</v>
       </c>
       <c r="I10" s="17">
@@ -1198,7 +1195,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="17">
-        <f>E10+H10+J10</f>
+        <f t="shared" si="1"/>
         <v>135.6</v>
       </c>
       <c r="L10" s="35" t="s">
@@ -1228,7 +1225,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="20">
-        <f>E11*0.13</f>
+        <f t="shared" si="0"/>
         <v>4.3485000000000005</v>
       </c>
       <c r="I11" s="20">
@@ -1238,7 +1235,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="20">
-        <f>E11+H11+J11</f>
+        <f t="shared" si="1"/>
         <v>37.798500000000004</v>
       </c>
       <c r="L11" s="34" t="s">
@@ -1268,7 +1265,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="17">
-        <f>E12*0.13</f>
+        <f t="shared" si="0"/>
         <v>268.85300000000001</v>
       </c>
       <c r="I12" s="17">
@@ -1278,7 +1275,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="38">
-        <f>E12+H12+J12</f>
+        <f t="shared" si="1"/>
         <v>2336.953</v>
       </c>
       <c r="L12" s="39" t="s">
@@ -1308,7 +1305,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="20">
-        <f>E13*0.13</f>
+        <f t="shared" si="0"/>
         <v>1.9487000000000001</v>
       </c>
       <c r="I13" s="20">
@@ -1322,21 +1319,21 @@
         <v>16.938700000000001</v>
       </c>
       <c r="L13" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="25.5">
       <c r="A14" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>57</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>58</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>47</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" s="17">
         <v>7.18</v>
@@ -1348,7 +1345,7 @@
         <v>1</v>
       </c>
       <c r="H14" s="17">
-        <f>E14*0.13</f>
+        <f t="shared" si="0"/>
         <v>0.93340000000000001</v>
       </c>
       <c r="I14" s="17">
@@ -1362,7 +1359,7 @@
         <v>8.1134000000000004</v>
       </c>
       <c r="L14" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75">
@@ -1378,7 +1375,7 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1393,11 +1390,11 @@
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="E17" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F17" s="27">
-        <f>SUM(K3:K12)</f>
-        <v>2710.1723999999999</v>
+        <f>SUM(K3:K14)</f>
+        <v>2735.2245000000003</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="7"/>
@@ -1409,11 +1406,10 @@
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="E18" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F18" s="27">
-        <f>SUM(K13:K14)</f>
-        <v>25.052100000000003</v>
+        <v>0</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="7"/>
@@ -1429,7 +1425,7 @@
       </c>
       <c r="F19" s="27">
         <f>F17+F18</f>
-        <v>2735.2244999999998</v>
+        <v>2735.2245000000003</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="7"/>

</xml_diff>